<commit_message>
Bug fixes on parameter variation, added parameters for surface, added ACF, PSD, RAPSD
</commit_message>
<xml_diff>
--- a/RCWA/Rebuild/layers.xlsx
+++ b/RCWA/Rebuild/layers.xlsx
@@ -384,8 +384,8 @@
       <c r="G2" s="1">
         <v>0.005</v>
       </c>
-      <c r="H2" s="2">
-        <v>0.0</v>
+      <c r="H2" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -410,8 +410,8 @@
       <c r="G3" s="1">
         <v>0.005</v>
       </c>
-      <c r="H3" s="2">
-        <v>0.0</v>
+      <c r="H3" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -436,8 +436,8 @@
       <c r="G4" s="1">
         <v>0.005</v>
       </c>
-      <c r="H4" s="2">
-        <v>0.0</v>
+      <c r="H4" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -445,13 +445,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="1">
-        <v>500.0</v>
+        <v>300.0</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5" s="3">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="E5" s="2">
         <v>0.0</v>
@@ -462,8 +462,8 @@
       <c r="G5" s="1">
         <v>0.005</v>
       </c>
-      <c r="H5" s="2">
-        <v>0.0</v>
+      <c r="H5" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -488,8 +488,8 @@
       <c r="G6" s="1">
         <v>0.005</v>
       </c>
-      <c r="H6" s="2">
-        <v>0.0</v>
+      <c r="H6" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -514,8 +514,8 @@
       <c r="G7" s="1">
         <v>0.005</v>
       </c>
-      <c r="H7" s="2">
-        <v>0.0</v>
+      <c r="H7" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -540,8 +540,8 @@
       <c r="G8" s="1">
         <v>0.005</v>
       </c>
-      <c r="H8" s="2">
-        <v>0.0</v>
+      <c r="H8" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -552,10 +552,10 @@
         <v>250.0</v>
       </c>
       <c r="C9" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>40.0</v>
       </c>
       <c r="E9" s="2">
         <v>0.0</v>
@@ -566,8 +566,8 @@
       <c r="G9" s="1">
         <v>0.005</v>
       </c>
-      <c r="H9" s="2">
-        <v>0.0</v>
+      <c r="H9" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
@@ -592,8 +592,8 @@
       <c r="G10" s="1">
         <v>0.005</v>
       </c>
-      <c r="H10" s="2">
-        <v>0.0</v>
+      <c r="H10" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">

</xml_diff>